<commit_message>
Aircraft generator klaar, begonnen met berekeningen
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofma\Documents\runway-allocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8CCB5E-9962-4CF7-A2FB-24D3EB2B3EE1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4F7D32-A4E9-4225-A5C7-3DD1A6ACC9BA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R06_Arr_M" sheetId="2" r:id="rId1"/>
@@ -19,13 +19,15 @@
     <sheet name="R24_Arr_H" sheetId="5" r:id="rId4"/>
     <sheet name="t_to_RWY" sheetId="6" r:id="rId5"/>
     <sheet name="t_to_taxi" sheetId="7" r:id="rId6"/>
+    <sheet name="fuel_flow" sheetId="8" r:id="rId7"/>
+    <sheet name="sound" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
   <si>
     <t>Nr</t>
   </si>
@@ -52,6 +54,18 @@
   </si>
   <si>
     <t>RIVER</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Taxi</t>
+  </si>
+  <si>
+    <t>Landing</t>
   </si>
 </sst>
 </file>
@@ -381,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -644,6 +658,19 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -697,7 +724,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -720,6 +747,14 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2058,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F2F097-6CC4-41B6-9082-1BF6A7A2B098}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2170,4 +2205,96 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B1FDC2-733F-4FC5-A603-DD7E80AB7F0B}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6"/>
+      <c r="B1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.22</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="15">
+        <v>0.12</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D7B831-465F-4D9E-A34C-BDBE150D7D37}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19"/>
+      <c r="B1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Missing: constraint 2 en time limit
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luka\Documents\runway-allocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F1BFC7-3CB0-4B28-AB2E-16CC92F5275D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C92837-7EAD-4251-BE74-3D6B9659984B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R06_Arr_M" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <sheet name="sound" sheetId="9" r:id="rId8"/>
     <sheet name="flights" sheetId="11" r:id="rId9"/>
     <sheet name="testset" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
@@ -1447,7 +1446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6572479F-AFDE-4940-94F1-052247087792}">
   <dimension ref="A1:T281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N145" sqref="N145"/>
     </sheetView>
   </sheetViews>
@@ -3285,7 +3284,7 @@
         <v>1</v>
       </c>
       <c r="P44" s="30">
-        <f ca="1">P16</f>
+        <f t="shared" ref="P44:P71" ca="1" si="0">P16</f>
         <v>270.53999999999996</v>
       </c>
     </row>
@@ -3326,7 +3325,7 @@
         <v>2</v>
       </c>
       <c r="P45" s="33">
-        <f ca="1">P17</f>
+        <f t="shared" ca="1" si="0"/>
         <v>274.94</v>
       </c>
     </row>
@@ -3367,7 +3366,7 @@
         <v>3</v>
       </c>
       <c r="P46" s="33">
-        <f ca="1">P18</f>
+        <f t="shared" ca="1" si="0"/>
         <v>279.33999999999997</v>
       </c>
     </row>
@@ -3408,7 +3407,7 @@
         <v>4</v>
       </c>
       <c r="P47" s="33">
-        <f ca="1">P19</f>
+        <f t="shared" ca="1" si="0"/>
         <v>283.74</v>
       </c>
     </row>
@@ -3449,7 +3448,7 @@
         <v>5</v>
       </c>
       <c r="P48" s="33">
-        <f ca="1">P20</f>
+        <f t="shared" ca="1" si="0"/>
         <v>288.14</v>
       </c>
     </row>
@@ -3490,7 +3489,7 @@
         <v>6</v>
       </c>
       <c r="P49" s="33">
-        <f ca="1">P21</f>
+        <f t="shared" ca="1" si="0"/>
         <v>292.53999999999996</v>
       </c>
     </row>
@@ -3531,7 +3530,7 @@
         <v>7</v>
       </c>
       <c r="P50" s="44">
-        <f>P22</f>
+        <f t="shared" si="0"/>
         <v>266.14</v>
       </c>
     </row>
@@ -3572,7 +3571,7 @@
         <v>1</v>
       </c>
       <c r="P51" s="33">
-        <f ca="1">P23</f>
+        <f t="shared" ca="1" si="0"/>
         <v>119.74000000000001</v>
       </c>
     </row>
@@ -3613,7 +3612,7 @@
         <v>2</v>
       </c>
       <c r="P52" s="33">
-        <f ca="1">P24</f>
+        <f t="shared" ca="1" si="0"/>
         <v>124.14</v>
       </c>
     </row>
@@ -3654,7 +3653,7 @@
         <v>3</v>
       </c>
       <c r="P53" s="33">
-        <f ca="1">P25</f>
+        <f t="shared" ca="1" si="0"/>
         <v>128.54</v>
       </c>
     </row>
@@ -3695,7 +3694,7 @@
         <v>4</v>
       </c>
       <c r="P54" s="33">
-        <f ca="1">P26</f>
+        <f t="shared" ca="1" si="0"/>
         <v>132.94</v>
       </c>
     </row>
@@ -3736,7 +3735,7 @@
         <v>5</v>
       </c>
       <c r="P55" s="33">
-        <f ca="1">P27</f>
+        <f t="shared" ca="1" si="0"/>
         <v>137.34</v>
       </c>
     </row>
@@ -3777,7 +3776,7 @@
         <v>6</v>
       </c>
       <c r="P56" s="33">
-        <f ca="1">P28</f>
+        <f t="shared" ca="1" si="0"/>
         <v>141.74</v>
       </c>
     </row>
@@ -3817,7 +3816,7 @@
         <v>7</v>
       </c>
       <c r="P57" s="36">
-        <f>P29</f>
+        <f t="shared" si="0"/>
         <v>115.34</v>
       </c>
     </row>
@@ -3858,7 +3857,7 @@
         <v>1</v>
       </c>
       <c r="P58" s="47">
-        <f ca="1">P30</f>
+        <f t="shared" ca="1" si="0"/>
         <v>398.07000000000005</v>
       </c>
     </row>
@@ -3899,7 +3898,7 @@
         <v>2</v>
       </c>
       <c r="P59" s="47">
-        <f ca="1">P31</f>
+        <f t="shared" ca="1" si="0"/>
         <v>408.67</v>
       </c>
     </row>
@@ -3940,7 +3939,7 @@
         <v>3</v>
       </c>
       <c r="P60" s="47">
-        <f ca="1">P32</f>
+        <f t="shared" ca="1" si="0"/>
         <v>419.27000000000004</v>
       </c>
     </row>
@@ -3981,7 +3980,7 @@
         <v>4</v>
       </c>
       <c r="P61" s="47">
-        <f ca="1">P33</f>
+        <f t="shared" ca="1" si="0"/>
         <v>429.87</v>
       </c>
     </row>
@@ -4022,7 +4021,7 @@
         <v>5</v>
       </c>
       <c r="P62" s="47">
-        <f ca="1">P34</f>
+        <f t="shared" ca="1" si="0"/>
         <v>440.47</v>
       </c>
     </row>
@@ -4063,7 +4062,7 @@
         <v>6</v>
       </c>
       <c r="P63" s="47">
-        <f ca="1">P35</f>
+        <f t="shared" ca="1" si="0"/>
         <v>451.07000000000005</v>
       </c>
     </row>
@@ -4104,7 +4103,7 @@
         <v>7</v>
       </c>
       <c r="P64" s="48">
-        <f>P36</f>
+        <f t="shared" si="0"/>
         <v>387.47</v>
       </c>
     </row>
@@ -4145,7 +4144,7 @@
         <v>1</v>
       </c>
       <c r="P65" s="47">
-        <f ca="1">P37</f>
+        <f t="shared" ca="1" si="0"/>
         <v>573.50000000000011</v>
       </c>
     </row>
@@ -4186,7 +4185,7 @@
         <v>2</v>
       </c>
       <c r="P66" s="47">
-        <f ca="1">P38</f>
+        <f t="shared" ca="1" si="0"/>
         <v>584.10000000000014</v>
       </c>
     </row>
@@ -4227,7 +4226,7 @@
         <v>3</v>
       </c>
       <c r="P67" s="47">
-        <f ca="1">P39</f>
+        <f t="shared" ca="1" si="0"/>
         <v>594.70000000000005</v>
       </c>
     </row>
@@ -4268,7 +4267,7 @@
         <v>4</v>
       </c>
       <c r="P68" s="47">
-        <f ca="1">P40</f>
+        <f t="shared" ca="1" si="0"/>
         <v>605.30000000000007</v>
       </c>
     </row>
@@ -4309,7 +4308,7 @@
         <v>5</v>
       </c>
       <c r="P69" s="47">
-        <f ca="1">P41</f>
+        <f t="shared" ca="1" si="0"/>
         <v>615.90000000000009</v>
       </c>
     </row>
@@ -4350,7 +4349,7 @@
         <v>6</v>
       </c>
       <c r="P70" s="47">
-        <f ca="1">P42</f>
+        <f t="shared" ca="1" si="0"/>
         <v>626.50000000000011</v>
       </c>
     </row>
@@ -4390,7 +4389,7 @@
         <v>7</v>
       </c>
       <c r="P71" s="53">
-        <f>P43</f>
+        <f t="shared" si="0"/>
         <v>562.90000000000009</v>
       </c>
     </row>
@@ -4431,7 +4430,7 @@
         <v>1</v>
       </c>
       <c r="P72" s="47">
-        <f>P2</f>
+        <f t="shared" ref="P72:P77" si="1">P2</f>
         <v>151.51999999999998</v>
       </c>
     </row>
@@ -4472,7 +4471,7 @@
         <v>2</v>
       </c>
       <c r="P73" s="47">
-        <f>P3</f>
+        <f t="shared" si="1"/>
         <v>155.91999999999999</v>
       </c>
     </row>
@@ -4513,7 +4512,7 @@
         <v>3</v>
       </c>
       <c r="P74" s="47">
-        <f>P4</f>
+        <f t="shared" si="1"/>
         <v>160.31999999999996</v>
       </c>
     </row>
@@ -4554,7 +4553,7 @@
         <v>4</v>
       </c>
       <c r="P75" s="47">
-        <f>P5</f>
+        <f t="shared" si="1"/>
         <v>164.71999999999997</v>
       </c>
     </row>
@@ -4595,7 +4594,7 @@
         <v>5</v>
       </c>
       <c r="P76" s="47">
-        <f>P6</f>
+        <f t="shared" si="1"/>
         <v>169.11999999999998</v>
       </c>
     </row>
@@ -4636,7 +4635,7 @@
         <v>6</v>
       </c>
       <c r="P77" s="47">
-        <f>P7</f>
+        <f t="shared" si="1"/>
         <v>173.51999999999998</v>
       </c>
     </row>
@@ -4717,7 +4716,7 @@
         <v>1</v>
       </c>
       <c r="P79" s="47">
-        <f ca="1">P9</f>
+        <f t="shared" ref="P79:P84" ca="1" si="2">P9</f>
         <v>268.02</v>
       </c>
     </row>
@@ -4758,7 +4757,7 @@
         <v>2</v>
       </c>
       <c r="P80" s="47">
-        <f ca="1">P10</f>
+        <f t="shared" ca="1" si="2"/>
         <v>272.42</v>
       </c>
     </row>
@@ -4799,7 +4798,7 @@
         <v>3</v>
       </c>
       <c r="P81" s="47">
-        <f ca="1">P11</f>
+        <f t="shared" ca="1" si="2"/>
         <v>276.82</v>
       </c>
     </row>
@@ -4840,7 +4839,7 @@
         <v>4</v>
       </c>
       <c r="P82" s="47">
-        <f ca="1">P12</f>
+        <f t="shared" ca="1" si="2"/>
         <v>281.22000000000003</v>
       </c>
     </row>
@@ -4881,7 +4880,7 @@
         <v>5</v>
       </c>
       <c r="P83" s="47">
-        <f ca="1">P13</f>
+        <f t="shared" ca="1" si="2"/>
         <v>285.62</v>
       </c>
     </row>
@@ -4922,7 +4921,7 @@
         <v>6</v>
       </c>
       <c r="P84" s="47">
-        <f ca="1">P14</f>
+        <f t="shared" ca="1" si="2"/>
         <v>290.02</v>
       </c>
     </row>
@@ -4989,7 +4988,7 @@
         <v>1</v>
       </c>
       <c r="J86" s="30">
-        <f t="shared" ref="J86:J112" si="0">J30</f>
+        <f t="shared" ref="J86:J112" si="3">J30</f>
         <v>270.53999999999996</v>
       </c>
       <c r="M86" s="45">
@@ -5017,7 +5016,7 @@
         <v>1</v>
       </c>
       <c r="D87" s="33">
-        <f t="shared" ref="D87:D113" si="1">D31</f>
+        <f t="shared" ref="D87:D113" si="4">D31</f>
         <v>270.53999999999996</v>
       </c>
       <c r="G87" s="45">
@@ -5030,7 +5029,7 @@
         <v>2</v>
       </c>
       <c r="J87" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>274.94</v>
       </c>
       <c r="M87" s="45">
@@ -5058,7 +5057,7 @@
         <v>2</v>
       </c>
       <c r="D88" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>274.94</v>
       </c>
       <c r="G88" s="45">
@@ -5071,7 +5070,7 @@
         <v>3</v>
       </c>
       <c r="J88" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>279.33999999999997</v>
       </c>
       <c r="M88" s="45">
@@ -5099,7 +5098,7 @@
         <v>3</v>
       </c>
       <c r="D89" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>279.33999999999997</v>
       </c>
       <c r="G89" s="45">
@@ -5112,7 +5111,7 @@
         <v>4</v>
       </c>
       <c r="J89" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>283.74</v>
       </c>
       <c r="M89" s="45">
@@ -5140,7 +5139,7 @@
         <v>4</v>
       </c>
       <c r="D90" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>283.74</v>
       </c>
       <c r="G90" s="45">
@@ -5153,7 +5152,7 @@
         <v>5</v>
       </c>
       <c r="J90" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>288.14</v>
       </c>
       <c r="M90" s="45">
@@ -5181,7 +5180,7 @@
         <v>5</v>
       </c>
       <c r="D91" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>288.14</v>
       </c>
       <c r="G91" s="45">
@@ -5194,7 +5193,7 @@
         <v>6</v>
       </c>
       <c r="J91" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>292.53999999999996</v>
       </c>
       <c r="M91" s="45">
@@ -5222,7 +5221,7 @@
         <v>6</v>
       </c>
       <c r="D92" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>292.53999999999996</v>
       </c>
       <c r="G92" s="45">
@@ -5235,7 +5234,7 @@
         <v>7</v>
       </c>
       <c r="J92" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>296.94</v>
       </c>
       <c r="M92" s="43">
@@ -5262,7 +5261,7 @@
         <v>7</v>
       </c>
       <c r="D93" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>296.94</v>
       </c>
       <c r="G93" s="45">
@@ -5275,7 +5274,7 @@
         <v>8</v>
       </c>
       <c r="J93" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>301.33999999999997</v>
       </c>
       <c r="M93" s="45">
@@ -5303,7 +5302,7 @@
         <v>8</v>
       </c>
       <c r="D94" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>301.33999999999997</v>
       </c>
       <c r="G94" s="45">
@@ -5316,7 +5315,7 @@
         <v>9</v>
       </c>
       <c r="J94" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>305.74</v>
       </c>
       <c r="M94" s="45">
@@ -5344,7 +5343,7 @@
         <v>9</v>
       </c>
       <c r="D95" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>305.74</v>
       </c>
       <c r="G95" s="45">
@@ -5357,7 +5356,7 @@
         <v>10</v>
       </c>
       <c r="J95" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>310.14</v>
       </c>
       <c r="M95" s="45">
@@ -5385,7 +5384,7 @@
         <v>10</v>
       </c>
       <c r="D96" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>310.14</v>
       </c>
       <c r="G96" s="45">
@@ -5398,7 +5397,7 @@
         <v>11</v>
       </c>
       <c r="J96" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>314.53999999999996</v>
       </c>
       <c r="M96" s="45">
@@ -5426,7 +5425,7 @@
         <v>11</v>
       </c>
       <c r="D97" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>314.53999999999996</v>
       </c>
       <c r="G97" s="45">
@@ -5439,7 +5438,7 @@
         <v>12</v>
       </c>
       <c r="J97" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>318.94</v>
       </c>
       <c r="M97" s="45">
@@ -5467,7 +5466,7 @@
         <v>12</v>
       </c>
       <c r="D98" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>318.94</v>
       </c>
       <c r="G98" s="45">
@@ -5480,7 +5479,7 @@
         <v>13</v>
       </c>
       <c r="J98" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>323.33999999999997</v>
       </c>
       <c r="M98" s="45">
@@ -5508,7 +5507,7 @@
         <v>13</v>
       </c>
       <c r="D99" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>323.33999999999997</v>
       </c>
       <c r="G99" s="43">
@@ -5521,7 +5520,7 @@
         <v>14</v>
       </c>
       <c r="J99" s="44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>266.14</v>
       </c>
       <c r="M99" s="34">
@@ -5548,7 +5547,7 @@
         <v>0</v>
       </c>
       <c r="D100" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>115.34</v>
       </c>
       <c r="G100" s="45">
@@ -5561,7 +5560,7 @@
         <v>1</v>
       </c>
       <c r="J100" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>119.74000000000001</v>
       </c>
       <c r="M100" s="45">
@@ -5589,7 +5588,7 @@
         <v>1</v>
       </c>
       <c r="D101" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>119.74000000000001</v>
       </c>
       <c r="G101" s="45">
@@ -5602,7 +5601,7 @@
         <v>2</v>
       </c>
       <c r="J101" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>124.14</v>
       </c>
       <c r="M101" s="45">
@@ -5630,7 +5629,7 @@
         <v>2</v>
       </c>
       <c r="D102" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>124.14</v>
       </c>
       <c r="G102" s="45">
@@ -5643,7 +5642,7 @@
         <v>3</v>
       </c>
       <c r="J102" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>128.54</v>
       </c>
       <c r="M102" s="45">
@@ -5671,7 +5670,7 @@
         <v>3</v>
       </c>
       <c r="D103" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>128.54</v>
       </c>
       <c r="G103" s="45">
@@ -5684,7 +5683,7 @@
         <v>4</v>
       </c>
       <c r="J103" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>132.94</v>
       </c>
       <c r="M103" s="45">
@@ -5712,7 +5711,7 @@
         <v>4</v>
       </c>
       <c r="D104" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>132.94</v>
       </c>
       <c r="G104" s="45">
@@ -5725,7 +5724,7 @@
         <v>5</v>
       </c>
       <c r="J104" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>137.34</v>
       </c>
       <c r="M104" s="45">
@@ -5753,7 +5752,7 @@
         <v>5</v>
       </c>
       <c r="D105" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>137.34</v>
       </c>
       <c r="G105" s="45">
@@ -5766,7 +5765,7 @@
         <v>6</v>
       </c>
       <c r="J105" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>141.74</v>
       </c>
       <c r="M105" s="45">
@@ -5794,7 +5793,7 @@
         <v>6</v>
       </c>
       <c r="D106" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>141.74</v>
       </c>
       <c r="G106" s="45">
@@ -5807,7 +5806,7 @@
         <v>7</v>
       </c>
       <c r="J106" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>146.14000000000001</v>
       </c>
       <c r="M106" s="43">
@@ -5834,7 +5833,7 @@
         <v>7</v>
       </c>
       <c r="D107" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>146.14000000000001</v>
       </c>
       <c r="G107" s="45">
@@ -5847,7 +5846,7 @@
         <v>8</v>
       </c>
       <c r="J107" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>150.54000000000002</v>
       </c>
       <c r="M107" s="45">
@@ -5875,7 +5874,7 @@
         <v>8</v>
       </c>
       <c r="D108" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>150.54000000000002</v>
       </c>
       <c r="G108" s="45">
@@ -5888,7 +5887,7 @@
         <v>9</v>
       </c>
       <c r="J108" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>154.94</v>
       </c>
       <c r="M108" s="45">
@@ -5916,7 +5915,7 @@
         <v>9</v>
       </c>
       <c r="D109" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>154.94</v>
       </c>
       <c r="G109" s="45">
@@ -5929,7 +5928,7 @@
         <v>10</v>
       </c>
       <c r="J109" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>159.34</v>
       </c>
       <c r="M109" s="45">
@@ -5957,7 +5956,7 @@
         <v>10</v>
       </c>
       <c r="D110" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>159.34</v>
       </c>
       <c r="G110" s="45">
@@ -5970,7 +5969,7 @@
         <v>11</v>
       </c>
       <c r="J110" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>163.74</v>
       </c>
       <c r="M110" s="45">
@@ -5998,7 +5997,7 @@
         <v>11</v>
       </c>
       <c r="D111" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>163.74</v>
       </c>
       <c r="G111" s="45">
@@ -6011,7 +6010,7 @@
         <v>12</v>
       </c>
       <c r="J111" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>168.14</v>
       </c>
       <c r="M111" s="45">
@@ -6039,7 +6038,7 @@
         <v>12</v>
       </c>
       <c r="D112" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>168.14</v>
       </c>
       <c r="G112" s="45">
@@ -6052,7 +6051,7 @@
         <v>13</v>
       </c>
       <c r="J112" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>172.54000000000002</v>
       </c>
       <c r="M112" s="45">
@@ -6080,7 +6079,7 @@
         <v>13</v>
       </c>
       <c r="D113" s="44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>172.54000000000002</v>
       </c>
       <c r="G113" s="34">
@@ -6093,7 +6092,7 @@
         <v>14</v>
       </c>
       <c r="J113" s="36">
-        <f t="shared" ref="J113" si="2">J57</f>
+        <f t="shared" ref="J113" si="5">J57</f>
         <v>115.34</v>
       </c>
       <c r="M113" s="34">
@@ -6133,7 +6132,7 @@
         <v>1</v>
       </c>
       <c r="J114" s="47">
-        <f t="shared" ref="J114:J140" si="3">J58</f>
+        <f t="shared" ref="J114:J140" si="6">J58</f>
         <v>398.07000000000005</v>
       </c>
       <c r="M114" s="45">
@@ -6161,7 +6160,7 @@
         <v>1</v>
       </c>
       <c r="D115" s="47">
-        <f t="shared" ref="D115:D141" si="4">D59</f>
+        <f t="shared" ref="D115:D141" si="7">D59</f>
         <v>398.07000000000005</v>
       </c>
       <c r="G115" s="45">
@@ -6174,7 +6173,7 @@
         <v>2</v>
       </c>
       <c r="J115" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>408.67</v>
       </c>
       <c r="M115" s="45">
@@ -6202,7 +6201,7 @@
         <v>2</v>
       </c>
       <c r="D116" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>408.67</v>
       </c>
       <c r="G116" s="45">
@@ -6215,7 +6214,7 @@
         <v>3</v>
       </c>
       <c r="J116" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>419.27000000000004</v>
       </c>
       <c r="M116" s="45">
@@ -6243,7 +6242,7 @@
         <v>3</v>
       </c>
       <c r="D117" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>419.27000000000004</v>
       </c>
       <c r="G117" s="45">
@@ -6256,7 +6255,7 @@
         <v>4</v>
       </c>
       <c r="J117" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>429.87</v>
       </c>
       <c r="M117" s="45">
@@ -6284,7 +6283,7 @@
         <v>4</v>
       </c>
       <c r="D118" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>429.87</v>
       </c>
       <c r="G118" s="45">
@@ -6297,7 +6296,7 @@
         <v>5</v>
       </c>
       <c r="J118" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>440.47</v>
       </c>
       <c r="M118" s="45">
@@ -6325,7 +6324,7 @@
         <v>5</v>
       </c>
       <c r="D119" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>440.47</v>
       </c>
       <c r="G119" s="45">
@@ -6338,7 +6337,7 @@
         <v>6</v>
       </c>
       <c r="J119" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>451.07000000000005</v>
       </c>
       <c r="M119" s="45">
@@ -6366,7 +6365,7 @@
         <v>6</v>
       </c>
       <c r="D120" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>451.07000000000005</v>
       </c>
       <c r="G120" s="45">
@@ -6379,7 +6378,7 @@
         <v>7</v>
       </c>
       <c r="J120" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>461.67</v>
       </c>
       <c r="M120" s="43">
@@ -6406,7 +6405,7 @@
         <v>7</v>
       </c>
       <c r="D121" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>461.67</v>
       </c>
       <c r="G121" s="45">
@@ -6419,7 +6418,7 @@
         <v>8</v>
       </c>
       <c r="J121" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>472.27000000000004</v>
       </c>
       <c r="M121" s="45">
@@ -6447,7 +6446,7 @@
         <v>8</v>
       </c>
       <c r="D122" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>472.27000000000004</v>
       </c>
       <c r="G122" s="45">
@@ -6460,7 +6459,7 @@
         <v>9</v>
       </c>
       <c r="J122" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>482.87</v>
       </c>
       <c r="M122" s="45">
@@ -6488,7 +6487,7 @@
         <v>9</v>
       </c>
       <c r="D123" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>482.87</v>
       </c>
       <c r="G123" s="45">
@@ -6501,7 +6500,7 @@
         <v>10</v>
       </c>
       <c r="J123" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>493.47</v>
       </c>
       <c r="M123" s="45">
@@ -6529,7 +6528,7 @@
         <v>10</v>
       </c>
       <c r="D124" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>493.47</v>
       </c>
       <c r="G124" s="45">
@@ -6542,7 +6541,7 @@
         <v>11</v>
       </c>
       <c r="J124" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>504.07000000000005</v>
       </c>
       <c r="M124" s="45">
@@ -6570,7 +6569,7 @@
         <v>11</v>
       </c>
       <c r="D125" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>504.07000000000005</v>
       </c>
       <c r="G125" s="45">
@@ -6583,7 +6582,7 @@
         <v>12</v>
       </c>
       <c r="J125" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>514.67000000000007</v>
       </c>
       <c r="M125" s="45">
@@ -6611,7 +6610,7 @@
         <v>12</v>
       </c>
       <c r="D126" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>514.67000000000007</v>
       </c>
       <c r="G126" s="45">
@@ -6624,7 +6623,7 @@
         <v>13</v>
       </c>
       <c r="J126" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>525.27</v>
       </c>
       <c r="M126" s="45">
@@ -6652,7 +6651,7 @@
         <v>13</v>
       </c>
       <c r="D127" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>525.27</v>
       </c>
       <c r="G127" s="43">
@@ -6665,7 +6664,7 @@
         <v>14</v>
       </c>
       <c r="J127" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>387.47</v>
       </c>
       <c r="M127" s="34">
@@ -6692,7 +6691,7 @@
         <v>0</v>
       </c>
       <c r="D128" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>562.90000000000009</v>
       </c>
       <c r="G128" s="45">
@@ -6705,7 +6704,7 @@
         <v>1</v>
       </c>
       <c r="J128" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>573.50000000000011</v>
       </c>
       <c r="M128" s="45">
@@ -6718,7 +6717,7 @@
         <v>1</v>
       </c>
       <c r="P128" s="33">
-        <f ca="1">P44</f>
+        <f t="shared" ref="P128:P140" ca="1" si="8">P44</f>
         <v>270.53999999999996</v>
       </c>
     </row>
@@ -6733,7 +6732,7 @@
         <v>1</v>
       </c>
       <c r="D129" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>573.50000000000011</v>
       </c>
       <c r="G129" s="45">
@@ -6746,7 +6745,7 @@
         <v>2</v>
       </c>
       <c r="J129" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>584.10000000000014</v>
       </c>
       <c r="M129" s="45">
@@ -6759,7 +6758,7 @@
         <v>2</v>
       </c>
       <c r="P129" s="33">
-        <f ca="1">P45</f>
+        <f t="shared" ca="1" si="8"/>
         <v>274.94</v>
       </c>
     </row>
@@ -6774,7 +6773,7 @@
         <v>2</v>
       </c>
       <c r="D130" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>584.10000000000014</v>
       </c>
       <c r="G130" s="45">
@@ -6787,7 +6786,7 @@
         <v>3</v>
       </c>
       <c r="J130" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>594.70000000000005</v>
       </c>
       <c r="M130" s="45">
@@ -6800,7 +6799,7 @@
         <v>3</v>
       </c>
       <c r="P130" s="33">
-        <f ca="1">P46</f>
+        <f t="shared" ca="1" si="8"/>
         <v>279.33999999999997</v>
       </c>
     </row>
@@ -6815,7 +6814,7 @@
         <v>3</v>
       </c>
       <c r="D131" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>594.70000000000005</v>
       </c>
       <c r="G131" s="45">
@@ -6828,7 +6827,7 @@
         <v>4</v>
       </c>
       <c r="J131" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>605.30000000000007</v>
       </c>
       <c r="M131" s="45">
@@ -6841,7 +6840,7 @@
         <v>4</v>
       </c>
       <c r="P131" s="33">
-        <f ca="1">P47</f>
+        <f t="shared" ca="1" si="8"/>
         <v>283.74</v>
       </c>
     </row>
@@ -6856,7 +6855,7 @@
         <v>4</v>
       </c>
       <c r="D132" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>605.30000000000007</v>
       </c>
       <c r="G132" s="45">
@@ -6869,7 +6868,7 @@
         <v>5</v>
       </c>
       <c r="J132" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>615.90000000000009</v>
       </c>
       <c r="M132" s="45">
@@ -6882,7 +6881,7 @@
         <v>5</v>
       </c>
       <c r="P132" s="33">
-        <f ca="1">P48</f>
+        <f t="shared" ca="1" si="8"/>
         <v>288.14</v>
       </c>
     </row>
@@ -6897,7 +6896,7 @@
         <v>5</v>
       </c>
       <c r="D133" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>615.90000000000009</v>
       </c>
       <c r="G133" s="45">
@@ -6910,7 +6909,7 @@
         <v>6</v>
       </c>
       <c r="J133" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>626.50000000000011</v>
       </c>
       <c r="M133" s="45">
@@ -6923,7 +6922,7 @@
         <v>6</v>
       </c>
       <c r="P133" s="33">
-        <f ca="1">P49</f>
+        <f t="shared" ca="1" si="8"/>
         <v>292.53999999999996</v>
       </c>
     </row>
@@ -6938,7 +6937,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>626.50000000000011</v>
       </c>
       <c r="G134" s="45">
@@ -6951,7 +6950,7 @@
         <v>7</v>
       </c>
       <c r="J134" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>637.10000000000014</v>
       </c>
       <c r="M134" s="43">
@@ -6964,7 +6963,7 @@
         <v>7</v>
       </c>
       <c r="P134" s="44">
-        <f>P50</f>
+        <f t="shared" si="8"/>
         <v>266.14</v>
       </c>
     </row>
@@ -6979,7 +6978,7 @@
         <v>7</v>
       </c>
       <c r="D135" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>637.10000000000014</v>
       </c>
       <c r="G135" s="45">
@@ -6992,7 +6991,7 @@
         <v>8</v>
       </c>
       <c r="J135" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>647.70000000000005</v>
       </c>
       <c r="M135" s="45">
@@ -7005,7 +7004,7 @@
         <v>1</v>
       </c>
       <c r="P135" s="33">
-        <f ca="1">P51</f>
+        <f t="shared" ca="1" si="8"/>
         <v>119.74000000000001</v>
       </c>
     </row>
@@ -7020,7 +7019,7 @@
         <v>8</v>
       </c>
       <c r="D136" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>647.70000000000005</v>
       </c>
       <c r="G136" s="45">
@@ -7033,7 +7032,7 @@
         <v>9</v>
       </c>
       <c r="J136" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>658.30000000000007</v>
       </c>
       <c r="M136" s="45">
@@ -7046,7 +7045,7 @@
         <v>2</v>
       </c>
       <c r="P136" s="33">
-        <f ca="1">P52</f>
+        <f t="shared" ca="1" si="8"/>
         <v>124.14</v>
       </c>
     </row>
@@ -7061,7 +7060,7 @@
         <v>9</v>
       </c>
       <c r="D137" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>658.30000000000007</v>
       </c>
       <c r="G137" s="45">
@@ -7074,7 +7073,7 @@
         <v>10</v>
       </c>
       <c r="J137" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>668.90000000000009</v>
       </c>
       <c r="M137" s="45">
@@ -7087,7 +7086,7 @@
         <v>3</v>
       </c>
       <c r="P137" s="33">
-        <f ca="1">P53</f>
+        <f t="shared" ca="1" si="8"/>
         <v>128.54</v>
       </c>
     </row>
@@ -7102,7 +7101,7 @@
         <v>10</v>
       </c>
       <c r="D138" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>668.90000000000009</v>
       </c>
       <c r="G138" s="45">
@@ -7115,7 +7114,7 @@
         <v>11</v>
       </c>
       <c r="J138" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>679.50000000000011</v>
       </c>
       <c r="M138" s="45">
@@ -7128,7 +7127,7 @@
         <v>4</v>
       </c>
       <c r="P138" s="33">
-        <f ca="1">P54</f>
+        <f t="shared" ca="1" si="8"/>
         <v>132.94</v>
       </c>
     </row>
@@ -7143,7 +7142,7 @@
         <v>11</v>
       </c>
       <c r="D139" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>679.50000000000011</v>
       </c>
       <c r="G139" s="45">
@@ -7156,7 +7155,7 @@
         <v>12</v>
       </c>
       <c r="J139" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>690.10000000000014</v>
       </c>
       <c r="M139" s="45">
@@ -7169,7 +7168,7 @@
         <v>5</v>
       </c>
       <c r="P139" s="33">
-        <f ca="1">P55</f>
+        <f t="shared" ca="1" si="8"/>
         <v>137.34</v>
       </c>
     </row>
@@ -7184,7 +7183,7 @@
         <v>12</v>
       </c>
       <c r="D140" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>690.10000000000014</v>
       </c>
       <c r="G140" s="45">
@@ -7197,7 +7196,7 @@
         <v>13</v>
       </c>
       <c r="J140" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>700.7</v>
       </c>
       <c r="M140" s="45">
@@ -7210,7 +7209,7 @@
         <v>6</v>
       </c>
       <c r="P140" s="33">
-        <f ca="1">P56</f>
+        <f t="shared" ca="1" si="8"/>
         <v>141.74</v>
       </c>
     </row>
@@ -7225,7 +7224,7 @@
         <v>13</v>
       </c>
       <c r="D141" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>700.7</v>
       </c>
       <c r="G141" s="34">
@@ -7238,7 +7237,7 @@
         <v>14</v>
       </c>
       <c r="J141" s="53">
-        <f t="shared" ref="J141" si="5">J85</f>
+        <f t="shared" ref="J141" si="9">J85</f>
         <v>562.90000000000009</v>
       </c>
       <c r="M141" s="34">
@@ -7278,7 +7277,7 @@
         <v>1</v>
       </c>
       <c r="J142" s="47">
-        <f t="shared" ref="J142:J154" si="6">J2</f>
+        <f t="shared" ref="J142:J154" si="10">J2</f>
         <v>151.51999999999998</v>
       </c>
     </row>
@@ -7293,7 +7292,7 @@
         <v>1</v>
       </c>
       <c r="D143" s="47">
-        <f t="shared" ref="D143:D169" si="7">D3</f>
+        <f t="shared" ref="D143:D169" si="11">D3</f>
         <v>151.51999999999998</v>
       </c>
       <c r="G143" s="45">
@@ -7306,7 +7305,7 @@
         <v>2</v>
       </c>
       <c r="J143" s="47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>155.91999999999999</v>
       </c>
     </row>
@@ -7321,7 +7320,7 @@
         <v>2</v>
       </c>
       <c r="D144" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>155.91999999999999</v>
       </c>
       <c r="G144" s="45">
@@ -7334,7 +7333,7 @@
         <v>3</v>
       </c>
       <c r="J144" s="47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>160.31999999999996</v>
       </c>
     </row>
@@ -7349,7 +7348,7 @@
         <v>3</v>
       </c>
       <c r="D145" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>160.31999999999996</v>
       </c>
       <c r="G145" s="45">
@@ -7362,7 +7361,7 @@
         <v>4</v>
       </c>
       <c r="J145" s="47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>164.71999999999997</v>
       </c>
     </row>
@@ -7377,7 +7376,7 @@
         <v>4</v>
       </c>
       <c r="D146" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>164.71999999999997</v>
       </c>
       <c r="G146" s="45">
@@ -7390,7 +7389,7 @@
         <v>5</v>
       </c>
       <c r="J146" s="47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>169.11999999999998</v>
       </c>
     </row>
@@ -7405,7 +7404,7 @@
         <v>5</v>
       </c>
       <c r="D147" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>169.11999999999998</v>
       </c>
       <c r="G147" s="45">
@@ -7418,7 +7417,7 @@
         <v>6</v>
       </c>
       <c r="J147" s="47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>173.51999999999998</v>
       </c>
     </row>
@@ -7433,7 +7432,7 @@
         <v>6</v>
       </c>
       <c r="D148" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>173.51999999999998</v>
       </c>
       <c r="G148" s="45">
@@ -7446,7 +7445,7 @@
         <v>7</v>
       </c>
       <c r="J148" s="47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>177.92</v>
       </c>
     </row>
@@ -7461,7 +7460,7 @@
         <v>7</v>
       </c>
       <c r="D149" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>177.92</v>
       </c>
       <c r="G149" s="45">
@@ -7474,7 +7473,7 @@
         <v>8</v>
       </c>
       <c r="J149" s="47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>182.32</v>
       </c>
     </row>
@@ -7489,7 +7488,7 @@
         <v>8</v>
       </c>
       <c r="D150" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>182.32</v>
       </c>
       <c r="G150" s="45">
@@ -7502,7 +7501,7 @@
         <v>9</v>
       </c>
       <c r="J150" s="47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>186.71999999999997</v>
       </c>
     </row>
@@ -7517,7 +7516,7 @@
         <v>9</v>
       </c>
       <c r="D151" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>186.71999999999997</v>
       </c>
       <c r="G151" s="45">
@@ -7530,7 +7529,7 @@
         <v>10</v>
       </c>
       <c r="J151" s="47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>191.11999999999998</v>
       </c>
     </row>
@@ -7545,7 +7544,7 @@
         <v>10</v>
       </c>
       <c r="D152" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>191.11999999999998</v>
       </c>
       <c r="G152" s="45">
@@ -7558,7 +7557,7 @@
         <v>11</v>
       </c>
       <c r="J152" s="47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>195.51999999999998</v>
       </c>
     </row>
@@ -7573,7 +7572,7 @@
         <v>11</v>
       </c>
       <c r="D153" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>195.51999999999998</v>
       </c>
       <c r="G153" s="45">
@@ -7586,7 +7585,7 @@
         <v>12</v>
       </c>
       <c r="J153" s="47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>199.91999999999996</v>
       </c>
     </row>
@@ -7601,7 +7600,7 @@
         <v>12</v>
       </c>
       <c r="D154" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>199.91999999999996</v>
       </c>
       <c r="G154" s="45">
@@ -7614,7 +7613,7 @@
         <v>13</v>
       </c>
       <c r="J154" s="47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>204.32</v>
       </c>
     </row>
@@ -7629,7 +7628,7 @@
         <v>13</v>
       </c>
       <c r="D155" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>204.32</v>
       </c>
       <c r="G155" s="43">
@@ -7656,7 +7655,7 @@
         <v>0</v>
       </c>
       <c r="D156" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>263.62</v>
       </c>
       <c r="G156" s="45">
@@ -7669,7 +7668,7 @@
         <v>1</v>
       </c>
       <c r="J156" s="47">
-        <f t="shared" ref="J156:J168" si="8">J16</f>
+        <f t="shared" ref="J156:J168" si="12">J16</f>
         <v>268.02</v>
       </c>
     </row>
@@ -7684,7 +7683,7 @@
         <v>1</v>
       </c>
       <c r="D157" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>268.02</v>
       </c>
       <c r="G157" s="45">
@@ -7697,7 +7696,7 @@
         <v>2</v>
       </c>
       <c r="J157" s="47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>272.42</v>
       </c>
     </row>
@@ -7712,7 +7711,7 @@
         <v>2</v>
       </c>
       <c r="D158" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>272.42</v>
       </c>
       <c r="G158" s="45">
@@ -7725,7 +7724,7 @@
         <v>3</v>
       </c>
       <c r="J158" s="47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>276.82</v>
       </c>
     </row>
@@ -7740,7 +7739,7 @@
         <v>3</v>
       </c>
       <c r="D159" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>276.82</v>
       </c>
       <c r="G159" s="45">
@@ -7753,7 +7752,7 @@
         <v>4</v>
       </c>
       <c r="J159" s="47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>281.22000000000003</v>
       </c>
     </row>
@@ -7768,7 +7767,7 @@
         <v>4</v>
       </c>
       <c r="D160" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>281.22000000000003</v>
       </c>
       <c r="G160" s="45">
@@ -7781,7 +7780,7 @@
         <v>5</v>
       </c>
       <c r="J160" s="47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>285.62</v>
       </c>
     </row>
@@ -7796,7 +7795,7 @@
         <v>5</v>
       </c>
       <c r="D161" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>285.62</v>
       </c>
       <c r="G161" s="45">
@@ -7809,7 +7808,7 @@
         <v>6</v>
       </c>
       <c r="J161" s="47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>290.02</v>
       </c>
     </row>
@@ -7824,7 +7823,7 @@
         <v>6</v>
       </c>
       <c r="D162" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>290.02</v>
       </c>
       <c r="G162" s="45">
@@ -7837,7 +7836,7 @@
         <v>7</v>
       </c>
       <c r="J162" s="47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>294.42</v>
       </c>
     </row>
@@ -7852,7 +7851,7 @@
         <v>7</v>
       </c>
       <c r="D163" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>294.42</v>
       </c>
       <c r="G163" s="45">
@@ -7865,7 +7864,7 @@
         <v>8</v>
       </c>
       <c r="J163" s="47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>298.82</v>
       </c>
     </row>
@@ -7880,7 +7879,7 @@
         <v>8</v>
       </c>
       <c r="D164" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>298.82</v>
       </c>
       <c r="G164" s="45">
@@ -7893,7 +7892,7 @@
         <v>9</v>
       </c>
       <c r="J164" s="47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>303.22000000000003</v>
       </c>
     </row>
@@ -7908,7 +7907,7 @@
         <v>9</v>
       </c>
       <c r="D165" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>303.22000000000003</v>
       </c>
       <c r="G165" s="45">
@@ -7921,7 +7920,7 @@
         <v>10</v>
       </c>
       <c r="J165" s="47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>307.62</v>
       </c>
     </row>
@@ -7936,7 +7935,7 @@
         <v>10</v>
       </c>
       <c r="D166" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>307.62</v>
       </c>
       <c r="G166" s="45">
@@ -7949,7 +7948,7 @@
         <v>11</v>
       </c>
       <c r="J166" s="47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>312.02</v>
       </c>
     </row>
@@ -7964,7 +7963,7 @@
         <v>11</v>
       </c>
       <c r="D167" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>312.02</v>
       </c>
       <c r="G167" s="45">
@@ -7977,7 +7976,7 @@
         <v>12</v>
       </c>
       <c r="J167" s="47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>316.42</v>
       </c>
     </row>
@@ -7992,7 +7991,7 @@
         <v>12</v>
       </c>
       <c r="D168" s="47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>316.42</v>
       </c>
       <c r="G168" s="45">
@@ -8005,7 +8004,7 @@
         <v>13</v>
       </c>
       <c r="J168" s="47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>320.82</v>
       </c>
     </row>
@@ -8020,7 +8019,7 @@
         <v>13</v>
       </c>
       <c r="D169" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>320.82</v>
       </c>
       <c r="G169" s="34">
@@ -10406,7 +10405,7 @@
         <v>1</v>
       </c>
       <c r="J254" s="33">
-        <f t="shared" ref="J254:J280" si="9">J86</f>
+        <f t="shared" ref="J254:J280" si="13">J86</f>
         <v>270.53999999999996</v>
       </c>
     </row>
@@ -10421,7 +10420,7 @@
         <v>1</v>
       </c>
       <c r="D255" s="33">
-        <f t="shared" ref="D255:D281" si="10">D87</f>
+        <f t="shared" ref="D255:D281" si="14">D87</f>
         <v>270.53999999999996</v>
       </c>
       <c r="G255" s="45">
@@ -10434,7 +10433,7 @@
         <v>2</v>
       </c>
       <c r="J255" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>274.94</v>
       </c>
     </row>
@@ -10449,7 +10448,7 @@
         <v>2</v>
       </c>
       <c r="D256" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>274.94</v>
       </c>
       <c r="G256" s="45">
@@ -10462,7 +10461,7 @@
         <v>3</v>
       </c>
       <c r="J256" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>279.33999999999997</v>
       </c>
     </row>
@@ -10477,7 +10476,7 @@
         <v>3</v>
       </c>
       <c r="D257" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>279.33999999999997</v>
       </c>
       <c r="G257" s="45">
@@ -10490,7 +10489,7 @@
         <v>4</v>
       </c>
       <c r="J257" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>283.74</v>
       </c>
     </row>
@@ -10505,7 +10504,7 @@
         <v>4</v>
       </c>
       <c r="D258" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>283.74</v>
       </c>
       <c r="G258" s="45">
@@ -10518,7 +10517,7 @@
         <v>5</v>
       </c>
       <c r="J258" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>288.14</v>
       </c>
     </row>
@@ -10533,7 +10532,7 @@
         <v>5</v>
       </c>
       <c r="D259" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>288.14</v>
       </c>
       <c r="G259" s="45">
@@ -10546,7 +10545,7 @@
         <v>6</v>
       </c>
       <c r="J259" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>292.53999999999996</v>
       </c>
     </row>
@@ -10561,7 +10560,7 @@
         <v>6</v>
       </c>
       <c r="D260" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>292.53999999999996</v>
       </c>
       <c r="G260" s="45">
@@ -10574,7 +10573,7 @@
         <v>7</v>
       </c>
       <c r="J260" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>296.94</v>
       </c>
     </row>
@@ -10589,7 +10588,7 @@
         <v>7</v>
       </c>
       <c r="D261" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>296.94</v>
       </c>
       <c r="G261" s="45">
@@ -10602,7 +10601,7 @@
         <v>8</v>
       </c>
       <c r="J261" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>301.33999999999997</v>
       </c>
     </row>
@@ -10617,7 +10616,7 @@
         <v>8</v>
       </c>
       <c r="D262" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>301.33999999999997</v>
       </c>
       <c r="G262" s="45">
@@ -10630,7 +10629,7 @@
         <v>9</v>
       </c>
       <c r="J262" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>305.74</v>
       </c>
     </row>
@@ -10645,7 +10644,7 @@
         <v>9</v>
       </c>
       <c r="D263" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>305.74</v>
       </c>
       <c r="G263" s="45">
@@ -10658,7 +10657,7 @@
         <v>10</v>
       </c>
       <c r="J263" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>310.14</v>
       </c>
     </row>
@@ -10673,7 +10672,7 @@
         <v>10</v>
       </c>
       <c r="D264" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>310.14</v>
       </c>
       <c r="G264" s="45">
@@ -10686,7 +10685,7 @@
         <v>11</v>
       </c>
       <c r="J264" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>314.53999999999996</v>
       </c>
     </row>
@@ -10701,7 +10700,7 @@
         <v>11</v>
       </c>
       <c r="D265" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>314.53999999999996</v>
       </c>
       <c r="G265" s="45">
@@ -10714,7 +10713,7 @@
         <v>12</v>
       </c>
       <c r="J265" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>318.94</v>
       </c>
     </row>
@@ -10729,7 +10728,7 @@
         <v>12</v>
       </c>
       <c r="D266" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>318.94</v>
       </c>
       <c r="G266" s="45">
@@ -10742,7 +10741,7 @@
         <v>13</v>
       </c>
       <c r="J266" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>323.33999999999997</v>
       </c>
     </row>
@@ -10757,7 +10756,7 @@
         <v>13</v>
       </c>
       <c r="D267" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>323.33999999999997</v>
       </c>
       <c r="G267" s="43">
@@ -10770,7 +10769,7 @@
         <v>14</v>
       </c>
       <c r="J267" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>266.14</v>
       </c>
     </row>
@@ -10785,7 +10784,7 @@
         <v>0</v>
       </c>
       <c r="D268" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>115.34</v>
       </c>
       <c r="G268" s="45">
@@ -10798,7 +10797,7 @@
         <v>1</v>
       </c>
       <c r="J268" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>119.74000000000001</v>
       </c>
     </row>
@@ -10813,7 +10812,7 @@
         <v>1</v>
       </c>
       <c r="D269" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>119.74000000000001</v>
       </c>
       <c r="G269" s="45">
@@ -10826,7 +10825,7 @@
         <v>2</v>
       </c>
       <c r="J269" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>124.14</v>
       </c>
     </row>
@@ -10841,7 +10840,7 @@
         <v>2</v>
       </c>
       <c r="D270" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>124.14</v>
       </c>
       <c r="G270" s="45">
@@ -10854,7 +10853,7 @@
         <v>3</v>
       </c>
       <c r="J270" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>128.54</v>
       </c>
     </row>
@@ -10869,7 +10868,7 @@
         <v>3</v>
       </c>
       <c r="D271" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>128.54</v>
       </c>
       <c r="G271" s="45">
@@ -10882,7 +10881,7 @@
         <v>4</v>
       </c>
       <c r="J271" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>132.94</v>
       </c>
     </row>
@@ -10897,7 +10896,7 @@
         <v>4</v>
       </c>
       <c r="D272" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>132.94</v>
       </c>
       <c r="G272" s="45">
@@ -10910,7 +10909,7 @@
         <v>5</v>
       </c>
       <c r="J272" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>137.34</v>
       </c>
     </row>
@@ -10925,7 +10924,7 @@
         <v>5</v>
       </c>
       <c r="D273" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>137.34</v>
       </c>
       <c r="G273" s="45">
@@ -10938,7 +10937,7 @@
         <v>6</v>
       </c>
       <c r="J273" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>141.74</v>
       </c>
     </row>
@@ -10953,7 +10952,7 @@
         <v>6</v>
       </c>
       <c r="D274" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>141.74</v>
       </c>
       <c r="G274" s="45">
@@ -10966,7 +10965,7 @@
         <v>7</v>
       </c>
       <c r="J274" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>146.14000000000001</v>
       </c>
     </row>
@@ -10981,7 +10980,7 @@
         <v>7</v>
       </c>
       <c r="D275" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>146.14000000000001</v>
       </c>
       <c r="G275" s="45">
@@ -10994,7 +10993,7 @@
         <v>8</v>
       </c>
       <c r="J275" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>150.54000000000002</v>
       </c>
     </row>
@@ -11009,7 +11008,7 @@
         <v>8</v>
       </c>
       <c r="D276" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>150.54000000000002</v>
       </c>
       <c r="G276" s="45">
@@ -11022,7 +11021,7 @@
         <v>9</v>
       </c>
       <c r="J276" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>154.94</v>
       </c>
     </row>
@@ -11037,7 +11036,7 @@
         <v>9</v>
       </c>
       <c r="D277" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>154.94</v>
       </c>
       <c r="G277" s="45">
@@ -11050,7 +11049,7 @@
         <v>10</v>
       </c>
       <c r="J277" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>159.34</v>
       </c>
     </row>
@@ -11065,7 +11064,7 @@
         <v>10</v>
       </c>
       <c r="D278" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>159.34</v>
       </c>
       <c r="G278" s="45">
@@ -11078,7 +11077,7 @@
         <v>11</v>
       </c>
       <c r="J278" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>163.74</v>
       </c>
     </row>
@@ -11093,7 +11092,7 @@
         <v>11</v>
       </c>
       <c r="D279" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>163.74</v>
       </c>
       <c r="G279" s="45">
@@ -11106,7 +11105,7 @@
         <v>12</v>
       </c>
       <c r="J279" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>168.14</v>
       </c>
     </row>
@@ -11121,7 +11120,7 @@
         <v>12</v>
       </c>
       <c r="D280" s="33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>168.14</v>
       </c>
       <c r="G280" s="45">
@@ -11134,7 +11133,7 @@
         <v>13</v>
       </c>
       <c r="J280" s="33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>172.54000000000002</v>
       </c>
     </row>
@@ -11149,7 +11148,7 @@
         <v>13</v>
       </c>
       <c r="D281" s="36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>172.54000000000002</v>
       </c>
       <c r="G281" s="34">
@@ -11164,813 +11163,6 @@
       <c r="J281" s="36">
         <v>115.34</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A2B5EA-9344-4738-B2C7-75215DBEDF9E}">
-  <dimension ref="A147:F245"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D141"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A147" s="32"/>
-      <c r="B147" s="32"/>
-      <c r="C147" s="32"/>
-      <c r="D147" s="32"/>
-      <c r="E147" s="32"/>
-      <c r="F147" s="32"/>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A148" s="32"/>
-      <c r="B148" s="32"/>
-      <c r="C148" s="32"/>
-      <c r="D148" s="32"/>
-      <c r="E148" s="32"/>
-      <c r="F148" s="32"/>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A149" s="32"/>
-      <c r="B149" s="32"/>
-      <c r="C149" s="32"/>
-      <c r="D149" s="32"/>
-      <c r="E149" s="32"/>
-      <c r="F149" s="32"/>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A150" s="32"/>
-      <c r="B150" s="32"/>
-      <c r="C150" s="32"/>
-      <c r="D150" s="32"/>
-      <c r="E150" s="32"/>
-      <c r="F150" s="32"/>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A151" s="32"/>
-      <c r="B151" s="32"/>
-      <c r="C151" s="32"/>
-      <c r="D151" s="32"/>
-      <c r="E151" s="32"/>
-      <c r="F151" s="32"/>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A152" s="32"/>
-      <c r="B152" s="32"/>
-      <c r="C152" s="32"/>
-      <c r="D152" s="32"/>
-      <c r="E152" s="32"/>
-      <c r="F152" s="32"/>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A153" s="32"/>
-      <c r="B153" s="32"/>
-      <c r="C153" s="32"/>
-      <c r="D153" s="32"/>
-      <c r="E153" s="32"/>
-      <c r="F153" s="32"/>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A154" s="32"/>
-      <c r="B154" s="32"/>
-      <c r="C154" s="32"/>
-      <c r="D154" s="32"/>
-      <c r="E154" s="32"/>
-      <c r="F154" s="32"/>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A155" s="32"/>
-      <c r="B155" s="32"/>
-      <c r="C155" s="32"/>
-      <c r="D155" s="32"/>
-      <c r="E155" s="32"/>
-      <c r="F155" s="32"/>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A156" s="41"/>
-      <c r="B156" s="41"/>
-      <c r="C156" s="41"/>
-      <c r="D156" s="32"/>
-      <c r="E156" s="32"/>
-      <c r="F156" s="32"/>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A157" s="41"/>
-      <c r="B157" s="41"/>
-      <c r="C157" s="41"/>
-      <c r="D157" s="32"/>
-      <c r="E157" s="32"/>
-      <c r="F157" s="32"/>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A158" s="41"/>
-      <c r="B158" s="41"/>
-      <c r="C158" s="41"/>
-      <c r="D158" s="32"/>
-      <c r="E158" s="32"/>
-      <c r="F158" s="32"/>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A159" s="41"/>
-      <c r="B159" s="41"/>
-      <c r="C159" s="41"/>
-      <c r="D159" s="32"/>
-      <c r="E159" s="32"/>
-      <c r="F159" s="32"/>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A160" s="41"/>
-      <c r="B160" s="41"/>
-      <c r="C160" s="41"/>
-      <c r="D160" s="32"/>
-      <c r="E160" s="32"/>
-      <c r="F160" s="32"/>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A161" s="41"/>
-      <c r="B161" s="41"/>
-      <c r="C161" s="41"/>
-      <c r="D161" s="32"/>
-      <c r="E161" s="32"/>
-      <c r="F161" s="32"/>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A162" s="32"/>
-      <c r="B162" s="32"/>
-      <c r="C162" s="32"/>
-      <c r="D162" s="32"/>
-      <c r="E162" s="32"/>
-      <c r="F162" s="32"/>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A163" s="32"/>
-      <c r="B163" s="32"/>
-      <c r="C163" s="32"/>
-      <c r="D163" s="32"/>
-      <c r="E163" s="32"/>
-      <c r="F163" s="32"/>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A164" s="32"/>
-      <c r="B164" s="32"/>
-      <c r="C164" s="32"/>
-      <c r="D164" s="32"/>
-      <c r="E164" s="32"/>
-      <c r="F164" s="32"/>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A165" s="32"/>
-      <c r="B165" s="32"/>
-      <c r="C165" s="32"/>
-      <c r="D165" s="32"/>
-      <c r="E165" s="32"/>
-      <c r="F165" s="32"/>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A166" s="32"/>
-      <c r="B166" s="32"/>
-      <c r="C166" s="32"/>
-      <c r="D166" s="32"/>
-      <c r="E166" s="32"/>
-      <c r="F166" s="32"/>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A167" s="32"/>
-      <c r="B167" s="32"/>
-      <c r="C167" s="32"/>
-      <c r="D167" s="32"/>
-      <c r="E167" s="32"/>
-      <c r="F167" s="32"/>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A168" s="32"/>
-      <c r="B168" s="32"/>
-      <c r="C168" s="32"/>
-      <c r="D168" s="32"/>
-      <c r="E168" s="32"/>
-      <c r="F168" s="32"/>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A169" s="32"/>
-      <c r="B169" s="32"/>
-      <c r="C169" s="32"/>
-      <c r="D169" s="32"/>
-      <c r="E169" s="32"/>
-      <c r="F169" s="32"/>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A170" s="41"/>
-      <c r="B170" s="41"/>
-      <c r="C170" s="41"/>
-      <c r="D170" s="32"/>
-      <c r="E170" s="32"/>
-      <c r="F170" s="32"/>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A171" s="41"/>
-      <c r="B171" s="41"/>
-      <c r="C171" s="41"/>
-      <c r="D171" s="32"/>
-      <c r="E171" s="32"/>
-      <c r="F171" s="32"/>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A172" s="41"/>
-      <c r="B172" s="41"/>
-      <c r="C172" s="41"/>
-      <c r="D172" s="32"/>
-      <c r="E172" s="32"/>
-      <c r="F172" s="32"/>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A173" s="41"/>
-      <c r="B173" s="41"/>
-      <c r="C173" s="41"/>
-      <c r="D173" s="32"/>
-      <c r="E173" s="32"/>
-      <c r="F173" s="32"/>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A174" s="41"/>
-      <c r="B174" s="41"/>
-      <c r="C174" s="41"/>
-      <c r="D174" s="32"/>
-      <c r="E174" s="32"/>
-      <c r="F174" s="32"/>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A175" s="41"/>
-      <c r="B175" s="41"/>
-      <c r="C175" s="41"/>
-      <c r="D175" s="32"/>
-      <c r="E175" s="32"/>
-      <c r="F175" s="32"/>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A176" s="32"/>
-      <c r="B176" s="32"/>
-      <c r="C176" s="32"/>
-      <c r="D176" s="32"/>
-      <c r="E176" s="32"/>
-      <c r="F176" s="32"/>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A177" s="32"/>
-      <c r="B177" s="32"/>
-      <c r="C177" s="32"/>
-      <c r="D177" s="32"/>
-      <c r="E177" s="32"/>
-      <c r="F177" s="32"/>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A178" s="32"/>
-      <c r="B178" s="32"/>
-      <c r="C178" s="32"/>
-      <c r="D178" s="32"/>
-      <c r="E178" s="32"/>
-      <c r="F178" s="32"/>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A179" s="32"/>
-      <c r="B179" s="32"/>
-      <c r="C179" s="32"/>
-      <c r="D179" s="32"/>
-      <c r="E179" s="32"/>
-      <c r="F179" s="32"/>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A180" s="32"/>
-      <c r="B180" s="32"/>
-      <c r="C180" s="32"/>
-      <c r="D180" s="32"/>
-      <c r="E180" s="32"/>
-      <c r="F180" s="32"/>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A181" s="32"/>
-      <c r="B181" s="32"/>
-      <c r="C181" s="32"/>
-      <c r="D181" s="32"/>
-      <c r="E181" s="32"/>
-      <c r="F181" s="32"/>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A182" s="32"/>
-      <c r="B182" s="32"/>
-      <c r="C182" s="32"/>
-      <c r="D182" s="32"/>
-      <c r="E182" s="32"/>
-      <c r="F182" s="32"/>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A183" s="32"/>
-      <c r="B183" s="32"/>
-      <c r="C183" s="32"/>
-      <c r="D183" s="32"/>
-      <c r="E183" s="32"/>
-      <c r="F183" s="32"/>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A184" s="32"/>
-      <c r="B184" s="32"/>
-      <c r="C184" s="32"/>
-      <c r="D184" s="32"/>
-      <c r="E184" s="32"/>
-      <c r="F184" s="32"/>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A185" s="32"/>
-      <c r="B185" s="32"/>
-      <c r="C185" s="32"/>
-      <c r="D185" s="32"/>
-      <c r="E185" s="32"/>
-      <c r="F185" s="32"/>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A186" s="32"/>
-      <c r="B186" s="32"/>
-      <c r="C186" s="32"/>
-      <c r="D186" s="32"/>
-      <c r="E186" s="32"/>
-      <c r="F186" s="32"/>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A187" s="32"/>
-      <c r="B187" s="32"/>
-      <c r="C187" s="32"/>
-      <c r="D187" s="32"/>
-      <c r="E187" s="32"/>
-      <c r="F187" s="32"/>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A188" s="32"/>
-      <c r="B188" s="32"/>
-      <c r="C188" s="32"/>
-      <c r="D188" s="32"/>
-      <c r="E188" s="32"/>
-      <c r="F188" s="32"/>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A189" s="32"/>
-      <c r="B189" s="32"/>
-      <c r="C189" s="32"/>
-      <c r="D189" s="32"/>
-      <c r="E189" s="32"/>
-      <c r="F189" s="32"/>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A190" s="32"/>
-      <c r="B190" s="32"/>
-      <c r="C190" s="32"/>
-      <c r="D190" s="32"/>
-      <c r="E190" s="32"/>
-      <c r="F190" s="32"/>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A191" s="32"/>
-      <c r="B191" s="32"/>
-      <c r="C191" s="32"/>
-      <c r="D191" s="32"/>
-      <c r="E191" s="32"/>
-      <c r="F191" s="32"/>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A192" s="32"/>
-      <c r="B192" s="32"/>
-      <c r="C192" s="32"/>
-      <c r="D192" s="32"/>
-      <c r="E192" s="32"/>
-      <c r="F192" s="32"/>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A193" s="32"/>
-      <c r="B193" s="32"/>
-      <c r="C193" s="32"/>
-      <c r="D193" s="32"/>
-      <c r="E193" s="32"/>
-      <c r="F193" s="32"/>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A194" s="32"/>
-      <c r="B194" s="32"/>
-      <c r="C194" s="32"/>
-      <c r="D194" s="32"/>
-      <c r="E194" s="32"/>
-      <c r="F194" s="32"/>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A195" s="32"/>
-      <c r="B195" s="32"/>
-      <c r="C195" s="32"/>
-      <c r="D195" s="32"/>
-      <c r="E195" s="32"/>
-      <c r="F195" s="32"/>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A196" s="32"/>
-      <c r="B196" s="32"/>
-      <c r="C196" s="32"/>
-      <c r="D196" s="32"/>
-      <c r="E196" s="32"/>
-      <c r="F196" s="32"/>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A197" s="32"/>
-      <c r="B197" s="32"/>
-      <c r="C197" s="32"/>
-      <c r="D197" s="32"/>
-      <c r="E197" s="32"/>
-      <c r="F197" s="32"/>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A198" s="32"/>
-      <c r="B198" s="32"/>
-      <c r="C198" s="32"/>
-      <c r="D198" s="32"/>
-      <c r="E198" s="32"/>
-      <c r="F198" s="32"/>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A199" s="32"/>
-      <c r="B199" s="32"/>
-      <c r="C199" s="32"/>
-      <c r="D199" s="32"/>
-      <c r="E199" s="32"/>
-      <c r="F199" s="32"/>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A200" s="32"/>
-      <c r="B200" s="32"/>
-      <c r="C200" s="32"/>
-      <c r="D200" s="32"/>
-      <c r="E200" s="32"/>
-      <c r="F200" s="32"/>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A201" s="32"/>
-      <c r="B201" s="32"/>
-      <c r="C201" s="32"/>
-      <c r="D201" s="32"/>
-      <c r="E201" s="32"/>
-      <c r="F201" s="32"/>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A202" s="32"/>
-      <c r="B202" s="32"/>
-      <c r="C202" s="32"/>
-      <c r="D202" s="32"/>
-      <c r="E202" s="32"/>
-      <c r="F202" s="32"/>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A203" s="32"/>
-      <c r="B203" s="32"/>
-      <c r="C203" s="32"/>
-      <c r="D203" s="32"/>
-      <c r="E203" s="32"/>
-      <c r="F203" s="32"/>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A204" s="32"/>
-      <c r="B204" s="32"/>
-      <c r="C204" s="32"/>
-      <c r="D204" s="32"/>
-      <c r="E204" s="32"/>
-      <c r="F204" s="32"/>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A205" s="32"/>
-      <c r="B205" s="32"/>
-      <c r="C205" s="32"/>
-      <c r="D205" s="32"/>
-      <c r="E205" s="32"/>
-      <c r="F205" s="32"/>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A206" s="32"/>
-      <c r="B206" s="32"/>
-      <c r="C206" s="32"/>
-      <c r="D206" s="32"/>
-      <c r="E206" s="32"/>
-      <c r="F206" s="32"/>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A207" s="32"/>
-      <c r="B207" s="32"/>
-      <c r="C207" s="32"/>
-      <c r="D207" s="32"/>
-      <c r="E207" s="32"/>
-      <c r="F207" s="32"/>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A208" s="32"/>
-      <c r="B208" s="32"/>
-      <c r="C208" s="32"/>
-      <c r="D208" s="32"/>
-      <c r="E208" s="32"/>
-      <c r="F208" s="32"/>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A209" s="32"/>
-      <c r="B209" s="32"/>
-      <c r="C209" s="32"/>
-      <c r="D209" s="32"/>
-      <c r="E209" s="32"/>
-      <c r="F209" s="32"/>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A210" s="32"/>
-      <c r="B210" s="32"/>
-      <c r="C210" s="32"/>
-      <c r="D210" s="32"/>
-      <c r="E210" s="32"/>
-      <c r="F210" s="32"/>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A211" s="32"/>
-      <c r="B211" s="32"/>
-      <c r="C211" s="32"/>
-      <c r="D211" s="32"/>
-      <c r="E211" s="32"/>
-      <c r="F211" s="32"/>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A212" s="32"/>
-      <c r="B212" s="32"/>
-      <c r="C212" s="32"/>
-      <c r="D212" s="32"/>
-      <c r="E212" s="32"/>
-      <c r="F212" s="32"/>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A213" s="32"/>
-      <c r="B213" s="32"/>
-      <c r="C213" s="32"/>
-      <c r="D213" s="32"/>
-      <c r="E213" s="32"/>
-      <c r="F213" s="32"/>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A214" s="32"/>
-      <c r="B214" s="32"/>
-      <c r="C214" s="32"/>
-      <c r="D214" s="32"/>
-      <c r="E214" s="32"/>
-      <c r="F214" s="32"/>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A215" s="32"/>
-      <c r="B215" s="32"/>
-      <c r="C215" s="32"/>
-      <c r="D215" s="32"/>
-      <c r="E215" s="32"/>
-      <c r="F215" s="32"/>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A216" s="32"/>
-      <c r="B216" s="32"/>
-      <c r="C216" s="32"/>
-      <c r="D216" s="32"/>
-      <c r="E216" s="32"/>
-      <c r="F216" s="32"/>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A217" s="32"/>
-      <c r="B217" s="32"/>
-      <c r="C217" s="32"/>
-      <c r="D217" s="32"/>
-      <c r="E217" s="32"/>
-      <c r="F217" s="32"/>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A218" s="32"/>
-      <c r="B218" s="32"/>
-      <c r="C218" s="32"/>
-      <c r="D218" s="32"/>
-      <c r="E218" s="32"/>
-      <c r="F218" s="32"/>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A219" s="32"/>
-      <c r="B219" s="32"/>
-      <c r="C219" s="32"/>
-      <c r="D219" s="32"/>
-      <c r="E219" s="32"/>
-      <c r="F219" s="32"/>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A220" s="32"/>
-      <c r="B220" s="32"/>
-      <c r="C220" s="32"/>
-      <c r="D220" s="32"/>
-      <c r="E220" s="32"/>
-      <c r="F220" s="32"/>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A221" s="32"/>
-      <c r="B221" s="32"/>
-      <c r="C221" s="32"/>
-      <c r="D221" s="32"/>
-      <c r="E221" s="32"/>
-      <c r="F221" s="32"/>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A222" s="32"/>
-      <c r="B222" s="32"/>
-      <c r="C222" s="32"/>
-      <c r="D222" s="32"/>
-      <c r="E222" s="32"/>
-      <c r="F222" s="32"/>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A223" s="32"/>
-      <c r="B223" s="32"/>
-      <c r="C223" s="32"/>
-      <c r="D223" s="32"/>
-      <c r="E223" s="32"/>
-      <c r="F223" s="32"/>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A224" s="32"/>
-      <c r="B224" s="32"/>
-      <c r="C224" s="32"/>
-      <c r="D224" s="32"/>
-      <c r="E224" s="32"/>
-      <c r="F224" s="32"/>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A225" s="32"/>
-      <c r="B225" s="32"/>
-      <c r="C225" s="32"/>
-      <c r="D225" s="32"/>
-      <c r="E225" s="32"/>
-      <c r="F225" s="32"/>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A226" s="32"/>
-      <c r="B226" s="32"/>
-      <c r="C226" s="32"/>
-      <c r="D226" s="32"/>
-      <c r="E226" s="32"/>
-      <c r="F226" s="32"/>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A227" s="32"/>
-      <c r="B227" s="32"/>
-      <c r="C227" s="32"/>
-      <c r="D227" s="32"/>
-      <c r="E227" s="32"/>
-      <c r="F227" s="32"/>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A228" s="32"/>
-      <c r="B228" s="32"/>
-      <c r="C228" s="32"/>
-      <c r="D228" s="32"/>
-      <c r="E228" s="32"/>
-      <c r="F228" s="32"/>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A229" s="32"/>
-      <c r="B229" s="32"/>
-      <c r="C229" s="32"/>
-      <c r="D229" s="32"/>
-      <c r="E229" s="32"/>
-      <c r="F229" s="32"/>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A230" s="32"/>
-      <c r="B230" s="32"/>
-      <c r="C230" s="32"/>
-      <c r="D230" s="32"/>
-      <c r="E230" s="32"/>
-      <c r="F230" s="32"/>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A231" s="32"/>
-      <c r="B231" s="32"/>
-      <c r="C231" s="32"/>
-      <c r="D231" s="32"/>
-      <c r="E231" s="32"/>
-      <c r="F231" s="32"/>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A232" s="32"/>
-      <c r="B232" s="32"/>
-      <c r="C232" s="32"/>
-      <c r="D232" s="32"/>
-      <c r="E232" s="32"/>
-      <c r="F232" s="32"/>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A233" s="32"/>
-      <c r="B233" s="32"/>
-      <c r="C233" s="32"/>
-      <c r="D233" s="32"/>
-      <c r="E233" s="32"/>
-      <c r="F233" s="32"/>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A234" s="32"/>
-      <c r="B234" s="32"/>
-      <c r="C234" s="32"/>
-      <c r="D234" s="32"/>
-      <c r="E234" s="32"/>
-      <c r="F234" s="32"/>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A235" s="32"/>
-      <c r="B235" s="32"/>
-      <c r="C235" s="32"/>
-      <c r="D235" s="32"/>
-      <c r="E235" s="32"/>
-      <c r="F235" s="32"/>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A236" s="32"/>
-      <c r="B236" s="32"/>
-      <c r="C236" s="32"/>
-      <c r="D236" s="32"/>
-      <c r="E236" s="32"/>
-      <c r="F236" s="32"/>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A237" s="32"/>
-      <c r="B237" s="32"/>
-      <c r="C237" s="32"/>
-      <c r="D237" s="32"/>
-      <c r="E237" s="32"/>
-      <c r="F237" s="32"/>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A238" s="32"/>
-      <c r="B238" s="32"/>
-      <c r="C238" s="32"/>
-      <c r="D238" s="32"/>
-      <c r="E238" s="32"/>
-      <c r="F238" s="32"/>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A239" s="41"/>
-      <c r="B239" s="41"/>
-      <c r="C239" s="41"/>
-      <c r="D239" s="32"/>
-      <c r="E239" s="32"/>
-      <c r="F239" s="32"/>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A240" s="41"/>
-      <c r="B240" s="41"/>
-      <c r="C240" s="41"/>
-      <c r="D240" s="32"/>
-      <c r="E240" s="32"/>
-      <c r="F240" s="32"/>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A241" s="41"/>
-      <c r="B241" s="41"/>
-      <c r="C241" s="41"/>
-      <c r="D241" s="32"/>
-      <c r="E241" s="32"/>
-      <c r="F241" s="32"/>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A242" s="41"/>
-      <c r="B242" s="41"/>
-      <c r="C242" s="41"/>
-      <c r="D242" s="32"/>
-      <c r="E242" s="32"/>
-      <c r="F242" s="32"/>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A243" s="41"/>
-      <c r="B243" s="41"/>
-      <c r="C243" s="41"/>
-      <c r="D243" s="32"/>
-      <c r="E243" s="32"/>
-      <c r="F243" s="32"/>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A244" s="41"/>
-      <c r="B244" s="41"/>
-      <c r="C244" s="41"/>
-      <c r="D244" s="32"/>
-      <c r="E244" s="32"/>
-      <c r="F244" s="32"/>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A245" s="41"/>
-      <c r="B245" s="41"/>
-      <c r="C245" s="41"/>
-      <c r="D245" s="32"/>
-      <c r="E245" s="32"/>
-      <c r="F245" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12926,7 +12118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD6EA91-B2D9-460A-B72F-58023DD02AD7}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding christophes part (constraint 2)
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofma\Documents\runway-allocation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luka\Documents\runway-allocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D43927-4C1C-43BD-A5B9-164D281F82EB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722123BD-44B8-42C5-8A4B-F0B2C0A64AFE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R06_Arr_M" sheetId="2" r:id="rId1"/>
@@ -1596,7 +1596,7 @@
         <v>2</v>
       </c>
       <c r="P3" s="33">
-        <f t="shared" ref="P3:P8" si="0">J3</f>
+        <f t="shared" ref="P3:P7" si="0">J3</f>
         <v>156.80000000000001</v>
       </c>
       <c r="Q3" s="32"/>
@@ -1911,7 +1911,7 @@
         <v>2</v>
       </c>
       <c r="P10" s="33">
-        <f t="shared" ref="P10:P15" si="1">J17</f>
+        <f t="shared" ref="P10:P14" si="1">J17</f>
         <v>273.08000000000004</v>
       </c>
       <c r="Q10" s="32"/>
@@ -2217,7 +2217,7 @@
         <v>2</v>
       </c>
       <c r="P17" s="33">
-        <f t="shared" ref="P17:P22" si="2">J31</f>
+        <f t="shared" ref="P17:P21" si="2">J31</f>
         <v>275.60000000000002</v>
       </c>
       <c r="R17" s="41"/>
@@ -2511,7 +2511,7 @@
         <v>2</v>
       </c>
       <c r="P24" s="33">
-        <f t="shared" ref="P24:P29" si="3">J45</f>
+        <f t="shared" ref="P24:P28" si="3">J45</f>
         <v>123.48</v>
       </c>
       <c r="R24" s="41"/>
@@ -2804,7 +2804,7 @@
         <v>2</v>
       </c>
       <c r="P31" s="33">
-        <f t="shared" ref="P31:P36" si="4">J59</f>
+        <f t="shared" ref="P31:P35" si="4">J59</f>
         <v>410.2</v>
       </c>
     </row>
@@ -3091,7 +3091,7 @@
         <v>2</v>
       </c>
       <c r="P38" s="33">
-        <f t="shared" ref="P38:P43" si="5">J73</f>
+        <f t="shared" ref="P38:P42" si="5">J73</f>
         <v>584.10000000000014</v>
       </c>
     </row>
@@ -3378,7 +3378,7 @@
         <v>2</v>
       </c>
       <c r="P45" s="33">
-        <f t="shared" ref="P45:P50" si="6">J87</f>
+        <f t="shared" ref="P45:P49" si="6">J87</f>
         <v>275.60000000000002</v>
       </c>
     </row>
@@ -3665,7 +3665,7 @@
         <v>2</v>
       </c>
       <c r="P52" s="33">
-        <f t="shared" ref="P52:P57" si="7">J101</f>
+        <f t="shared" ref="P52:P56" si="7">J101</f>
         <v>123.48</v>
       </c>
     </row>
@@ -3952,7 +3952,7 @@
         <v>2</v>
       </c>
       <c r="P59" s="47">
-        <f t="shared" ref="P59:P64" si="8">J115</f>
+        <f t="shared" ref="P59:P63" si="8">J115</f>
         <v>410.2</v>
       </c>
     </row>
@@ -4239,7 +4239,7 @@
         <v>2</v>
       </c>
       <c r="P66" s="47">
-        <f t="shared" ref="P66:P71" si="9">J129</f>
+        <f t="shared" ref="P66:P70" si="9">J129</f>
         <v>584.10000000000014</v>
       </c>
     </row>
@@ -4526,7 +4526,7 @@
         <v>2</v>
       </c>
       <c r="P73" s="47">
-        <f t="shared" ref="P73:P78" si="10">J143</f>
+        <f t="shared" ref="P73:P77" si="10">J143</f>
         <v>156.80000000000001</v>
       </c>
     </row>
@@ -4813,7 +4813,7 @@
         <v>2</v>
       </c>
       <c r="P80" s="47">
-        <f t="shared" ref="P80:P85" si="11">J157</f>
+        <f t="shared" ref="P80:P84" si="11">J157</f>
         <v>273.08000000000004</v>
       </c>
     </row>
@@ -5100,7 +5100,7 @@
         <v>2</v>
       </c>
       <c r="P87" s="47">
-        <f t="shared" ref="P87:P92" si="14">J171</f>
+        <f t="shared" ref="P87:P91" si="14">J171</f>
         <v>664.6</v>
       </c>
     </row>
@@ -5387,7 +5387,7 @@
         <v>2</v>
       </c>
       <c r="P94" s="47">
-        <f t="shared" ref="P94:P99" si="15">J185</f>
+        <f t="shared" ref="P94:P98" si="15">J185</f>
         <v>297.89999999999998</v>
       </c>
     </row>
@@ -5674,7 +5674,7 @@
         <v>2</v>
       </c>
       <c r="P101" s="47">
-        <f t="shared" ref="P101:P106" si="17">J199</f>
+        <f t="shared" ref="P101:P105" si="17">J199</f>
         <v>378.40000000000003</v>
       </c>
     </row>
@@ -5961,7 +5961,7 @@
         <v>2</v>
       </c>
       <c r="P108" s="33">
-        <f t="shared" ref="P108:P113" si="18">J213</f>
+        <f t="shared" ref="P108:P112" si="18">J213</f>
         <v>658.30000000000007</v>
       </c>
     </row>
@@ -6248,7 +6248,7 @@
         <v>2</v>
       </c>
       <c r="P115" s="33">
-        <f t="shared" ref="P115:P120" si="22">J227</f>
+        <f t="shared" ref="P115:P119" si="22">J227</f>
         <v>170</v>
       </c>
     </row>
@@ -6535,7 +6535,7 @@
         <v>2</v>
       </c>
       <c r="P122" s="33">
-        <f t="shared" ref="P122:P127" si="23">J241</f>
+        <f t="shared" ref="P122:P126" si="23">J241</f>
         <v>242.28000000000003</v>
       </c>
     </row>
@@ -6822,7 +6822,7 @@
         <v>2</v>
       </c>
       <c r="P129" s="33">
-        <f t="shared" ref="P129:P134" si="24">J255</f>
+        <f t="shared" ref="P129:P133" si="24">J255</f>
         <v>275.60000000000002</v>
       </c>
     </row>
@@ -7109,7 +7109,7 @@
         <v>2</v>
       </c>
       <c r="P136" s="33">
-        <f t="shared" ref="P136:P141" si="25">J269</f>
+        <f t="shared" ref="P136:P140" si="25">J269</f>
         <v>123.48</v>
       </c>
     </row>
@@ -11247,7 +11247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F2A5A1-E880-4844-A90B-E2D712D9D7B7}">
   <dimension ref="A1:Z281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
@@ -23958,8 +23958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD6EA91-B2D9-460A-B72F-58023DD02AD7}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>